<commit_message>
Small fixes, moar templates
</commit_message>
<xml_diff>
--- a/API/Model/GenerateExcel/Templates/Faculty Details Report.xlsx
+++ b/API/Model/GenerateExcel/Templates/Faculty Details Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GC-FaMS-API\API\Model\GenerateExcel\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1909C736-C5FE-483A-ACC3-F58881A17D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE851DE-CD38-46EE-97E8-374BF26BC5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29655" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{9BFB484B-CCF6-4471-8DB9-57ECD0265C47}"/>
+    <workbookView xWindow="29625" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{9BFB484B-CCF6-4471-8DB9-57ECD0265C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -206,6 +206,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1211036</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3390E7EA-7E73-BBB9-5BCA-A217779E4C40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1877786" cy="1877786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,9 +585,7 @@
   </sheetPr>
   <dimension ref="A3:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1478,5 +1531,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>